<commit_message>
interpolated + 0-1 normalised heatmap, initial tracepeak graph, basic colour consistency
</commit_message>
<xml_diff>
--- a/ion_rhythmicity.xlsx
+++ b/ion_rhythmicity.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -363,25 +363,30 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>rowname</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Ion</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>pVal</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>phase</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>peak.shape</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>period</t>
         </is>
@@ -390,76 +395,96 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>4.189047761245855E-21</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>22</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Mg</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.004613852787293322</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>18</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Ca</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.004263315365191727</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>18</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>K</t>
         </is>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>1.345439998676246E-11</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>16</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>24</v>
       </c>
     </row>
@@ -470,7 +495,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,25 +504,30 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>rowname</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Ion</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>pVal</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>phase</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>peak.shape</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>period</t>
         </is>
@@ -506,76 +536,96 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>2.894257498096193E-45</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Mg</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>2.917243396018233E-31</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
       </c>
       <c r="D3">
         <v>12</v>
       </c>
       <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
         <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Ca</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.0001298639475702177</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>12</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>K</t>
         </is>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>2.760357753881839E-24</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>14</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>26</v>
       </c>
     </row>
@@ -2470,7 +2520,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.03662065632051746</v>
+        <v>0.03519532527725465</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -2478,412 +2528,412 @@
         </is>
       </c>
       <c r="F2">
-        <v>122.7574447631768</v>
+        <v>121.592002147231</v>
       </c>
       <c r="G2">
-        <v>0.2677244110089436</v>
+        <v>0.2707988810173659</v>
       </c>
       <c r="H2">
-        <v>23.46885472079604</v>
+        <v>23.20240498621801</v>
       </c>
       <c r="I2">
-        <v>0.7107197599563219</v>
+        <v>0.4156676061582751</v>
       </c>
       <c r="J2">
-        <v>20.81418547611301</v>
+        <v>21.66743702550616</v>
       </c>
       <c r="K2">
-        <v>-0.8121481460502606</v>
+        <v>-1.430924138269907</v>
       </c>
       <c r="L2">
-        <v>-0.05480429751538453</v>
+        <v>-0.05480429751538454</v>
       </c>
       <c r="M2">
-        <v>0.6425375829121168</v>
+        <v>0.6560776469198434</v>
       </c>
       <c r="N2">
-        <v>9.963064157595175E-21</v>
+        <v>1.525351862313161E-21</v>
       </c>
       <c r="O2">
-        <v>2.988919247278552E-20</v>
+        <v>4.576055586939484E-21</v>
       </c>
       <c r="P2">
-        <v>5.479685286677346E-20</v>
+        <v>8.389435242722387E-21</v>
       </c>
       <c r="Q2">
-        <v>33.4169233359539</v>
+        <v>31.9562009687808</v>
       </c>
       <c r="R2">
-        <v>33.3806249776154</v>
+        <v>35.0521718687808</v>
       </c>
       <c r="S2">
-        <v>21.0099093031231</v>
+        <v>21.1907873187808</v>
       </c>
       <c r="T2">
-        <v>42.3960766084307</v>
+        <v>42.0043740687807</v>
       </c>
       <c r="U2">
-        <v>39.5832658760077</v>
+        <v>38.1790031638115</v>
       </c>
       <c r="V2">
-        <v>36.7877277535807</v>
+        <v>38.4417402138115</v>
       </c>
       <c r="W2">
-        <v>29.2338564190462</v>
+        <v>29.3779196138115</v>
       </c>
       <c r="X2">
-        <v>37.6864127566116</v>
+        <v>37.2925998138116</v>
       </c>
       <c r="Y2">
-        <v>-30.3870679439384</v>
+        <v>-31.7348710011577</v>
       </c>
       <c r="Z2">
-        <v>-27.5351595154539</v>
+        <v>-25.8986814861577</v>
       </c>
       <c r="AA2">
-        <v>-25.9941419350307</v>
+        <v>-25.8868935611577</v>
       </c>
       <c r="AB2">
-        <v>-34.2717833952077</v>
+        <v>-34.6677067411577</v>
       </c>
       <c r="AC2">
-        <v>-20.0428660388846</v>
+        <v>-21.3342094411269</v>
       </c>
       <c r="AD2">
-        <v>-19.3707175644885</v>
+        <v>-17.7517739661269</v>
       </c>
       <c r="AE2">
-        <v>-13.7117459191077</v>
+        <v>-13.641312366127</v>
       </c>
       <c r="AF2">
-        <v>-28.0165138520269</v>
+        <v>-28.4145476011269</v>
       </c>
       <c r="AG2">
-        <v>-38.8528762088308</v>
+        <v>-40.0877599560962</v>
       </c>
       <c r="AH2">
-        <v>-39.0013520885231</v>
+        <v>-37.3999429210962</v>
       </c>
       <c r="AI2">
-        <v>-36.2534080731846</v>
+        <v>-36.2197893410961</v>
       </c>
       <c r="AJ2">
-        <v>-34.2825240738462</v>
+        <v>-34.6826682260962</v>
       </c>
       <c r="AK2">
-        <v>-44.7820141387769</v>
+        <v>-45.9604382310654</v>
       </c>
       <c r="AL2">
-        <v>-49.7699704275577</v>
+        <v>-48.1860956910654</v>
       </c>
       <c r="AM2">
-        <v>-36.2330546922615</v>
+        <v>-36.2362507810654</v>
       </c>
       <c r="AN2">
-        <v>-41.7837387006654</v>
+        <v>-42.1859932560654</v>
       </c>
       <c r="AO2">
-        <v>-36.2171569787231</v>
+        <v>-37.3391214160346</v>
       </c>
       <c r="AP2">
-        <v>-39.1545150565923</v>
+        <v>-37.5881747510346</v>
       </c>
       <c r="AQ2">
-        <v>-38.8354538613384</v>
+        <v>-38.8754647710346</v>
       </c>
       <c r="AR2">
-        <v>-31.6642172074846</v>
+        <v>-32.0685821660346</v>
       </c>
       <c r="AS2">
-        <v>24.6201477163308</v>
+        <v>23.5546429339961</v>
       </c>
       <c r="AT2">
-        <v>32.2939005093731</v>
+        <v>33.8427063839962</v>
       </c>
       <c r="AU2">
-        <v>31.9537437145846</v>
+        <v>31.8769179839962</v>
       </c>
       <c r="AV2">
-        <v>28.2414718456961</v>
+        <v>27.8349964839962</v>
       </c>
       <c r="AW2">
-        <v>33.0176892563846</v>
+        <v>32.0086441290269</v>
       </c>
       <c r="AX2">
-        <v>34.1474276853384</v>
+        <v>35.6786991290269</v>
       </c>
       <c r="AY2">
-        <v>39.2446218805077</v>
+        <v>39.130981329027</v>
       </c>
       <c r="AZ2">
-        <v>32.5421575938769</v>
+        <v>32.1335718290269</v>
       </c>
       <c r="BA2">
-        <v>30.3870800964385</v>
+        <v>29.4344946240577</v>
       </c>
       <c r="BB2">
-        <v>31.1564822613038</v>
+        <v>32.6702192740577</v>
       </c>
       <c r="BC2">
-        <v>36.5130902464308</v>
+        <v>36.3626348740577</v>
       </c>
       <c r="BD2">
-        <v>23.8382100420577</v>
+        <v>23.4275138740577</v>
       </c>
       <c r="BE2">
-        <v>45.7346363864923</v>
+        <v>44.8385105690884</v>
       </c>
       <c r="BF2">
-        <v>55.9437213372692</v>
+        <v>57.4399239190884</v>
       </c>
       <c r="BG2">
-        <v>42.2479623123539</v>
+        <v>42.0606921190885</v>
       </c>
       <c r="BH2">
-        <v>44.2538399402385</v>
+        <v>43.8410333690885</v>
       </c>
       <c r="BI2">
-        <v>64.1499697765462</v>
+        <v>63.3103036141192</v>
       </c>
       <c r="BJ2">
-        <v>55.0750885132346</v>
+        <v>56.5537566641192</v>
       </c>
       <c r="BK2">
-        <v>58.6403338282769</v>
+        <v>58.4162488141192</v>
       </c>
       <c r="BL2">
-        <v>52.8538371384192</v>
+        <v>52.4389201641192</v>
       </c>
       <c r="BM2">
-        <v>0.229393506600019</v>
+        <v>-0.553813000849971</v>
       </c>
       <c r="BN2">
-        <v>3.61401836420001</v>
+        <v>5.07515208415003</v>
       </c>
       <c r="BO2">
-        <v>4.55785442920001</v>
+        <v>4.29695459415001</v>
       </c>
       <c r="BP2">
-        <v>2.60236357159999</v>
+        <v>2.18533619415001</v>
       </c>
       <c r="BQ2">
-        <v>-5.29365648334613</v>
+        <v>-6.02040333581922</v>
       </c>
       <c r="BR2">
-        <v>-8.54154049483461</v>
+        <v>-7.09794120581921</v>
       </c>
       <c r="BS2">
-        <v>-3.04901715487691</v>
+        <v>-3.34673181081925</v>
       </c>
       <c r="BT2">
-        <v>-0.794490010219249</v>
+        <v>-1.21362779081926</v>
       </c>
       <c r="BU2">
-        <v>-19.2632529882923</v>
+        <v>-19.9335401857885</v>
       </c>
       <c r="BV2">
-        <v>-22.6214963388693</v>
+        <v>-21.1954314807885</v>
       </c>
       <c r="BW2">
-        <v>-19.4056401289538</v>
+        <v>-19.7401696057885</v>
       </c>
       <c r="BX2">
-        <v>-17.8615207070385</v>
+        <v>-18.2827688907884</v>
       </c>
       <c r="BY2">
-        <v>-29.8095145482385</v>
+        <v>-30.4233420907577</v>
       </c>
       <c r="BZ2">
-        <v>-32.3536522579039</v>
+        <v>-30.9451218307577</v>
       </c>
       <c r="CA2">
-        <v>-42.7217811080308</v>
+        <v>-43.0931254057577</v>
       </c>
       <c r="CB2">
-        <v>-39.9961439038577</v>
+        <v>-40.4195024907577</v>
       </c>
       <c r="CC2">
-        <v>-38.0450754531846</v>
+        <v>-38.6024433407269</v>
       </c>
       <c r="CD2">
-        <v>-46.2220087719385</v>
+        <v>-44.8310127757269</v>
       </c>
       <c r="CE2">
-        <v>-42.0783933571077</v>
+        <v>-42.4865524757269</v>
       </c>
       <c r="CF2">
-        <v>-31.9298845056769</v>
+        <v>-32.3553534957269</v>
       </c>
       <c r="CG2">
-        <v>-44.5462558631308</v>
+        <v>-45.0471640956962</v>
       </c>
       <c r="CH2">
-        <v>-32.6838528459731</v>
+        <v>-31.3103912806961</v>
       </c>
       <c r="CI2">
-        <v>-40.9490028261846</v>
+        <v>-41.3939767656962</v>
       </c>
       <c r="CJ2">
-        <v>-40.4194376524961</v>
+        <v>-40.8470170456961</v>
       </c>
       <c r="CK2">
-        <v>-27.4165597530769</v>
+        <v>-27.8610083306654</v>
       </c>
       <c r="CL2">
-        <v>-35.6623541100077</v>
+        <v>-34.3064269756654</v>
       </c>
       <c r="CM2">
-        <v>-32.4281944402615</v>
+        <v>-32.9099832006654</v>
       </c>
       <c r="CN2">
-        <v>-25.0518104243154</v>
+        <v>-25.4815002206654</v>
       </c>
       <c r="CO2">
-        <v>-2.41372068802306</v>
+        <v>-2.80170961063462</v>
       </c>
       <c r="CP2">
-        <v>4.95431828095764</v>
+        <v>6.29271098436536</v>
       </c>
       <c r="CQ2">
-        <v>2.83377701066158</v>
+        <v>2.31517342936539</v>
       </c>
       <c r="CR2">
-        <v>0.8708220688653801</v>
+        <v>0.439021869365376</v>
       </c>
       <c r="CS2">
-        <v>-1.32520305296919</v>
+        <v>-1.65673232060382</v>
       </c>
       <c r="CT2">
-        <v>-5.67746290807696</v>
+        <v>-4.35660463560384</v>
       </c>
       <c r="CU2">
-        <v>-5.68902849841538</v>
+        <v>-6.24444690060386</v>
       </c>
       <c r="CV2">
-        <v>-10.1812072279538</v>
+        <v>-10.6151178306038</v>
       </c>
       <c r="CW2">
-        <v>18.8845198770846</v>
+        <v>18.6094502644269</v>
       </c>
       <c r="CX2">
-        <v>19.4872571228884</v>
+        <v>20.7905809644269</v>
       </c>
       <c r="CY2">
-        <v>22.2026218375077</v>
+        <v>21.6103886144269</v>
       </c>
       <c r="CZ2">
-        <v>14.8304495602269</v>
+        <v>14.3944285544269</v>
       </c>
       <c r="DA2">
-        <v>20.4489537171385</v>
+        <v>20.2303437594577</v>
       </c>
       <c r="DB2">
-        <v>29.8156947488538</v>
+        <v>31.1014841594577</v>
       </c>
       <c r="DC2">
-        <v>17.9209173034308</v>
+        <v>17.2918692594577</v>
       </c>
       <c r="DD2">
-        <v>20.7878127184077</v>
+        <v>20.3496813094577</v>
       </c>
       <c r="DE2">
-        <v>-3.14987060280771</v>
+        <v>-3.31202090551156</v>
       </c>
       <c r="DF2">
-        <v>-5.77822072518077</v>
+        <v>-4.50996574551152</v>
       </c>
       <c r="DG2">
-        <v>4.49010592435388</v>
+        <v>3.82424305948848</v>
       </c>
       <c r="DH2">
-        <v>-2.39493929841154</v>
+        <v>-2.83518111051154</v>
       </c>
       <c r="DI2">
-        <v>31.0725111972461</v>
+        <v>30.9668205495192</v>
       </c>
       <c r="DJ2">
-        <v>27.7160415507846</v>
+        <v>28.9667620995193</v>
       </c>
       <c r="DK2">
-        <v>26.5000677852769</v>
+        <v>25.7973900995192</v>
       </c>
       <c r="DL2">
-        <v>37.7447571147692</v>
+        <v>37.3024048995192</v>
       </c>
       <c r="DM2">
-        <v>26.93814523801914</v>
+        <v>33.14365740522566</v>
       </c>
       <c r="DN2">
-        <v>1.16409620062002</v>
+        <v>7.67653003976028</v>
       </c>
       <c r="DO2">
-        <v>-23.32555505840818</v>
+        <v>-18.58713484557746</v>
       </c>
       <c r="DP2">
-        <v>-39.98119435421616</v>
+        <v>-38.30437030575165</v>
       </c>
       <c r="DQ2">
-        <v>-44.839941552873</v>
+        <v>-46.44811185059466</v>
       </c>
       <c r="DR2">
-        <v>-37.41749392730863</v>
+        <v>-41.54492128119181</v>
       </c>
       <c r="DS2">
-        <v>-20.59377473162225</v>
+        <v>-25.84236154182728</v>
       </c>
       <c r="DT2">
-        <v>0.405545868263171</v>
+        <v>-4.43232386047124</v>
       </c>
       <c r="DU2">
-        <v>19.59164619727213</v>
+        <v>16.3554298188169</v>
       </c>
       <c r="DV2">
-        <v>31.89030719332276</v>
+        <v>30.79407310604695</v>
       </c>
       <c r="DW2">
-        <v>34.4531849402814</v>
+        <v>35.30807144554021</v>
       </c>
       <c r="DX2">
-        <v>27.27293473491524</v>
+        <v>29.31925861515435</v>
       </c>
       <c r="DY2">
-        <v>12.98456137420916</v>
+        <v>15.20356018816009</v>
       </c>
       <c r="DZ2">
-        <v>-4.035669315592004</v>
+        <v>-2.569176080568751</v>
       </c>
       <c r="EA2">
-        <v>-18.97982060593026</v>
+        <v>-18.81799978535459</v>
       </c>
       <c r="EB2">
-        <v>-27.94243394937308</v>
+        <v>-29.13703550277311</v>
       </c>
       <c r="EC2">
-        <v>-28.91575056995318</v>
+        <v>-31.06554165643204</v>
       </c>
       <c r="ED2">
-        <v>-22.20008933555992</v>
+        <v>-24.63861662250653</v>
       </c>
       <c r="EE2">
-        <v>-10.15941141649828</v>
+        <v>-12.20781493673881</v>
       </c>
       <c r="EF2">
-        <v>3.565404907756687</v>
+        <v>2.36891842816106</v>
       </c>
       <c r="EG2">
-        <v>15.13396184972348</v>
+        <v>14.90031447963988</v>
       </c>
       <c r="EH2">
-        <v>21.56174949955268</v>
+        <v>22.04761866776271</v>
       </c>
       <c r="EI2">
-        <v>21.46894429579138</v>
+        <v>22.19323334431954</v>
       </c>
       <c r="EJ2">
-        <v>15.34121707107221</v>
+        <v>15.77265406334897</v>
       </c>
       <c r="EK2">
-        <v>5.266296638253319</v>
+        <v>5.01405917573411</v>
       </c>
     </row>
     <row r="3">
@@ -2899,15 +2949,15 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-0.1475693947720038</v>
+        <v>-0.1519227100023069</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Forced</t>
+          <t>Overexpressed</t>
         </is>
       </c>
       <c r="F3">
-        <v>0.004766089306384854</v>
+        <v>0.003463177229485598</v>
       </c>
       <c r="G3">
         <v>0.3141592653589793</v>
@@ -2916,403 +2966,403 @@
         <v>20</v>
       </c>
       <c r="I3">
-        <v>2.579476013161488</v>
+        <v>2.217076861929577</v>
       </c>
       <c r="J3">
-        <v>11.78927283836749</v>
+        <v>12.9428251641848</v>
       </c>
       <c r="K3">
-        <v>-0.4583116678370487</v>
+        <v>-1.852494636620293</v>
       </c>
       <c r="L3">
         <v>-0.01384460867601921</v>
       </c>
       <c r="M3">
-        <v>0.1472994842052682</v>
+        <v>0.1407346046863704</v>
       </c>
       <c r="N3">
-        <v>0.0323268679017121</v>
+        <v>0.04085940227600291</v>
       </c>
       <c r="O3">
-        <v>0.0323268679017121</v>
+        <v>0.04085940227600291</v>
       </c>
       <c r="P3">
-        <v>0.05926592448647219</v>
+        <v>0.074908904172672</v>
       </c>
       <c r="Q3">
-        <v>-1.05211404181169</v>
+        <v>-3.18205278826846</v>
       </c>
       <c r="R3">
-        <v>6.62091926552</v>
+        <v>5.57266969553154</v>
       </c>
       <c r="S3">
-        <v>-0.96887365126338</v>
+        <v>4.07871014413154</v>
       </c>
       <c r="T3">
-        <v>0.854183807481235</v>
+        <v>-1.01521167146846</v>
       </c>
       <c r="U3">
-        <v>4.47884139846262</v>
+        <v>2.50278640208358</v>
       </c>
       <c r="V3">
-        <v>-1.855649434022</v>
+        <v>-2.92657625011642</v>
       </c>
       <c r="W3">
-        <v>-5.90660479242277</v>
+        <v>-1.20401579451642</v>
       </c>
       <c r="X3">
-        <v>0.8715447061164669</v>
+        <v>-0.784062479316418</v>
       </c>
       <c r="Y3">
-        <v>-2.51638968686308</v>
+        <v>-4.33856093316438</v>
       </c>
       <c r="Z3">
-        <v>-2.052411934164</v>
+        <v>-3.14601599636438</v>
       </c>
       <c r="AA3">
-        <v>-7.08260283018215</v>
+        <v>-2.72500862976438</v>
       </c>
       <c r="AB3">
-        <v>-3.69056297944831</v>
+        <v>-5.13238187136438</v>
       </c>
       <c r="AC3">
-        <v>5.86051254901123</v>
+        <v>4.19222505278766</v>
       </c>
       <c r="AD3">
-        <v>-6.745409028106</v>
+        <v>-7.86169033641234</v>
       </c>
       <c r="AE3">
-        <v>20.2769511632585</v>
+        <v>24.2895505661876</v>
       </c>
       <c r="AF3">
-        <v>-3.55893970281308</v>
+        <v>-4.78697030121235</v>
       </c>
       <c r="AG3">
-        <v>-2.87708954731446</v>
+        <v>-4.3914932934603</v>
       </c>
       <c r="AH3">
-        <v>-0.342146527248001</v>
+        <v>-1.48110508166031</v>
       </c>
       <c r="AI3">
-        <v>-5.03726479250092</v>
+        <v>-1.3696601870603</v>
       </c>
       <c r="AJ3">
-        <v>2.82608998402215</v>
+        <v>1.8118476791397</v>
       </c>
       <c r="AK3">
-        <v>-2.54572156964015</v>
+        <v>-3.90624156570827</v>
       </c>
       <c r="AL3">
-        <v>-3.31400593459</v>
+        <v>-4.47564173510827</v>
       </c>
       <c r="AM3">
-        <v>2.8503407995397</v>
+        <v>6.17295060749174</v>
       </c>
       <c r="AN3">
-        <v>10.9150358408574</v>
+        <v>10.1145818294917</v>
       </c>
       <c r="AO3">
-        <v>3.24836597963415</v>
+        <v>2.04172973364377</v>
       </c>
       <c r="AP3">
-        <v>-0.528824961731999</v>
+        <v>-1.71313800835623</v>
       </c>
       <c r="AQ3">
-        <v>-2.37035705281969</v>
+        <v>0.607257957643768</v>
       </c>
       <c r="AR3">
-        <v>-2.89457337750738</v>
+        <v>-3.48123909535623</v>
       </c>
       <c r="AS3">
-        <v>-1.71705067089154</v>
+        <v>-2.76980316680419</v>
       </c>
       <c r="AT3">
-        <v>1.981212525526</v>
+        <v>0.774222232795807</v>
       </c>
       <c r="AU3">
-        <v>-1.72066993317907</v>
+        <v>0.911950279795807</v>
       </c>
       <c r="AV3">
-        <v>-0.968565861472154</v>
+        <v>-1.34144328580419</v>
       </c>
       <c r="AW3">
-        <v>0.810291121782768</v>
+        <v>-0.088577624052153</v>
       </c>
       <c r="AX3">
-        <v>0.718491451583997</v>
+        <v>-0.511176087252153</v>
       </c>
       <c r="AY3">
-        <v>2.06484014046154</v>
+        <v>4.35246555594785</v>
       </c>
       <c r="AZ3">
-        <v>-0.240373539236924</v>
+        <v>-0.399462670052152</v>
       </c>
       <c r="BA3">
-        <v>-0.960848811742924</v>
+        <v>-1.70583380750011</v>
       </c>
       <c r="BB3">
-        <v>2.904875042042</v>
+        <v>1.65253025709988</v>
       </c>
       <c r="BC3">
-        <v>2.50057486490216</v>
+        <v>4.44320548289989</v>
       </c>
       <c r="BD3">
-        <v>-1.02135838500169</v>
+        <v>-0.966659222300112</v>
       </c>
       <c r="BE3">
-        <v>0.930178582731383</v>
+        <v>0.339077337051922</v>
       </c>
       <c r="BF3">
-        <v>5.7025202729</v>
+        <v>4.42749824185192</v>
       </c>
       <c r="BG3">
-        <v>0.682547306142773</v>
+        <v>2.28018312665192</v>
       </c>
       <c r="BH3">
-        <v>1.55908279303354</v>
+        <v>1.82757024925192</v>
       </c>
       <c r="BI3">
-        <v>3.14069576980569</v>
+        <v>2.70347827420397</v>
       </c>
       <c r="BJ3">
-        <v>0.516728098758001</v>
+        <v>-0.780971178396033</v>
       </c>
       <c r="BK3">
-        <v>-0.0690848286166101</v>
+        <v>1.18355619440397</v>
       </c>
       <c r="BL3">
-        <v>-3.83209843953123</v>
+        <v>-3.34982268979604</v>
       </c>
       <c r="BM3">
-        <v>1.94363310828</v>
+        <v>1.660299362756</v>
       </c>
       <c r="BN3">
-        <v>2.765701501816</v>
+        <v>1.445324978556</v>
       </c>
       <c r="BO3">
-        <v>-2.97741834617599</v>
+        <v>-2.069772120644</v>
       </c>
       <c r="BP3">
-        <v>-4.872111407096</v>
+        <v>-4.176047363844</v>
       </c>
       <c r="BQ3">
-        <v>1.23559017935431</v>
+        <v>1.10614018390804</v>
       </c>
       <c r="BR3">
-        <v>-1.25287102372601</v>
+        <v>-2.59592479309196</v>
       </c>
       <c r="BS3">
-        <v>2.50385202446462</v>
+        <v>3.06650345250804</v>
       </c>
       <c r="BT3">
-        <v>0.9227817531392331</v>
+        <v>1.83263408990804</v>
       </c>
       <c r="BU3">
-        <v>-1.82054261357139</v>
+        <v>-1.79610885893992</v>
       </c>
       <c r="BV3">
-        <v>1.862712981132</v>
+        <v>0.496981965660083</v>
       </c>
       <c r="BW3">
-        <v>-1.69763824109477</v>
+        <v>-1.47998161053992</v>
       </c>
       <c r="BX3">
-        <v>5.46882840217446</v>
+        <v>6.59246903246008</v>
       </c>
       <c r="BY3">
-        <v>2.51508246890292</v>
+        <v>2.69339997361212</v>
       </c>
       <c r="BZ3">
-        <v>-2.56211820701</v>
+        <v>-3.95052646858788</v>
       </c>
       <c r="CA3">
-        <v>3.92944390914585</v>
+        <v>3.80210574221212</v>
       </c>
       <c r="CB3">
-        <v>-6.39872918579031</v>
+        <v>-5.06130026198788</v>
       </c>
       <c r="CC3">
-        <v>-5.56461521062277</v>
+        <v>-5.23241395583585</v>
       </c>
       <c r="CD3">
-        <v>-1.965444517752</v>
+        <v>-3.37653002543584</v>
       </c>
       <c r="CE3">
-        <v>-4.03596771861353</v>
+        <v>-4.50830068303584</v>
       </c>
       <c r="CF3">
-        <v>-4.80239928995508</v>
+        <v>-3.25118207263585</v>
       </c>
       <c r="CG3">
-        <v>-5.97683039814846</v>
+        <v>-5.49074539328381</v>
       </c>
       <c r="CH3">
-        <v>-1.928035271694</v>
+        <v>-3.36179802548381</v>
       </c>
       <c r="CI3">
-        <v>-3.46088980377292</v>
+        <v>-4.27821756568381</v>
       </c>
       <c r="CJ3">
-        <v>-5.04863540511985</v>
+        <v>-3.28362989428381</v>
       </c>
       <c r="CK3">
-        <v>-3.98535150447416</v>
+        <v>-3.34538274953177</v>
       </c>
       <c r="CL3">
-        <v>0.275145008563996</v>
+        <v>-1.18129499133177</v>
       </c>
       <c r="CM3">
-        <v>-2.0409796723323</v>
+        <v>-3.20330223173177</v>
       </c>
       <c r="CN3">
-        <v>-2.74011143368461</v>
+        <v>-0.7613176293317671</v>
       </c>
       <c r="CO3">
-        <v>-8.360034466199849</v>
+        <v>-7.56618196117973</v>
       </c>
       <c r="CP3">
-        <v>-2.404441575978</v>
+        <v>-3.88355882197973</v>
       </c>
       <c r="CQ3">
-        <v>-5.53571444689169</v>
+        <v>-7.04303180377973</v>
       </c>
       <c r="CR3">
-        <v>-8.719553542449381</v>
+        <v>-6.52697144457973</v>
       </c>
       <c r="CS3">
-        <v>-4.38211755712554</v>
+        <v>-3.43438130202769</v>
       </c>
       <c r="CT3">
-        <v>-2.37151305032</v>
+        <v>-3.87330754242769</v>
       </c>
       <c r="CU3">
-        <v>-0.946452106651076</v>
+        <v>-2.79876426102769</v>
       </c>
       <c r="CV3">
-        <v>47.1596539557858</v>
+        <v>49.5660243471723</v>
       </c>
       <c r="CW3">
-        <v>-4.33419321885123</v>
+        <v>-3.23257321367565</v>
       </c>
       <c r="CX3">
-        <v>2.001666493138</v>
+        <v>0.477194754924351</v>
       </c>
       <c r="CY3">
-        <v>7.82670494998954</v>
+        <v>5.62939799812435</v>
       </c>
       <c r="CZ3">
-        <v>-6.21880435057892</v>
+        <v>-3.59864566567565</v>
       </c>
       <c r="DA3">
-        <v>-0.285093773976925</v>
+        <v>0.970409981276386</v>
       </c>
       <c r="DB3">
-        <v>2.538988672196</v>
+        <v>0.991839687876389</v>
       </c>
       <c r="DC3">
-        <v>-0.0776558603698483</v>
+        <v>-2.61995760972362</v>
       </c>
       <c r="DD3">
-        <v>-5.71321726374369</v>
+        <v>-2.87927028532361</v>
       </c>
       <c r="DE3">
-        <v>20.5763459298974</v>
+        <v>21.9857334352284</v>
       </c>
       <c r="DF3">
-        <v>-2.37061798834601</v>
+        <v>-3.94044421877158</v>
       </c>
       <c r="DG3">
-        <v>-4.89336151492923</v>
+        <v>-7.78065806177158</v>
       </c>
       <c r="DH3">
-        <v>-6.34156103870846</v>
+        <v>-3.29382576677158</v>
       </c>
       <c r="DI3">
-        <v>1.63845598337169</v>
+        <v>3.20172723878046</v>
       </c>
       <c r="DJ3">
-        <v>1.804528141512</v>
+        <v>0.212024664980465</v>
       </c>
       <c r="DK3">
-        <v>6.18628043391139</v>
+        <v>2.95398908958046</v>
       </c>
       <c r="DL3">
-        <v>-3.51560604047323</v>
+        <v>-0.254082475019537</v>
       </c>
       <c r="DM3">
-        <v>-0.3972229177236093</v>
+        <v>-1.850110633420254</v>
       </c>
       <c r="DN3">
-        <v>-0.296945292980989</v>
+        <v>-1.759445866353062</v>
       </c>
       <c r="DO3">
-        <v>-0.2377587992190707</v>
+        <v>-1.680467255757013</v>
       </c>
       <c r="DP3">
-        <v>-0.2614691871452144</v>
+        <v>-1.654566788839399</v>
       </c>
       <c r="DQ3">
-        <v>-0.3854398103648582</v>
+        <v>-1.712803845936779</v>
       </c>
       <c r="DR3">
-        <v>-0.5860743759495668</v>
+        <v>-1.857590324363502</v>
       </c>
       <c r="DS3">
-        <v>-0.7957977845381752</v>
+        <v>-2.051381734659271</v>
       </c>
       <c r="DT3">
-        <v>-0.9195820609010961</v>
+        <v>-2.220194569299499</v>
       </c>
       <c r="DU3">
-        <v>-0.8699934972749409</v>
+        <v>-2.275555523434677</v>
       </c>
       <c r="DV3">
-        <v>-0.6107178938368906</v>
+        <v>-2.151076723218795</v>
       </c>
       <c r="DW3">
-        <v>-0.1911051927670389</v>
+        <v>-1.841602858632803</v>
       </c>
       <c r="DX3">
-        <v>0.24751616691231</v>
+        <v>-1.427383400300208</v>
       </c>
       <c r="DY3">
-        <v>0.5064020393603059</v>
+        <v>-1.066554399584733</v>
       </c>
       <c r="DZ3">
-        <v>0.402691140569244</v>
+        <v>-0.9482231257700147</v>
       </c>
       <c r="EA3">
-        <v>-0.1395650552317853</v>
+        <v>-1.214290342684425</v>
       </c>
       <c r="EB3">
-        <v>-1.017154708769294</v>
+        <v>-1.875775267951533</v>
       </c>
       <c r="EC3">
-        <v>-1.934499598696925</v>
+        <v>-2.76114866711036</v>
       </c>
       <c r="ED3">
-        <v>-2.475940700284487</v>
+        <v>-3.532402630322366</v>
       </c>
       <c r="EE3">
-        <v>-2.259036847026328</v>
+        <v>-3.78532981666427</v>
       </c>
       <c r="EF3">
-        <v>-1.124947183419188</v>
+        <v>-3.216624432343353</v>
       </c>
       <c r="EG3">
-        <v>0.7104681842102445</v>
+        <v>-1.802733450172714</v>
       </c>
       <c r="EH3">
-        <v>2.629028757027558</v>
+        <v>0.08970796021762251</v>
       </c>
       <c r="EI3">
-        <v>3.761413709965636</v>
+        <v>1.738224777299263</v>
       </c>
       <c r="EJ3">
-        <v>3.307774968939809</v>
+        <v>2.278844002703696</v>
       </c>
       <c r="EK3">
-        <v>0.9359083585442254</v>
+        <v>1.063264654348113</v>
       </c>
     </row>
     <row r="4">
@@ -3328,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.1358608462171936</v>
+        <v>0.1028698057222215</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -3336,412 +3386,412 @@
         </is>
       </c>
       <c r="F4">
-        <v>11198.02461218975</v>
+        <v>4390.170011636246</v>
       </c>
       <c r="G4">
-        <v>0.3021019652014981</v>
+        <v>0.2993416107211897</v>
       </c>
       <c r="H4">
-        <v>20.79822719123586</v>
+        <v>20.99001636305024</v>
       </c>
       <c r="I4">
-        <v>-1.265269131591427</v>
+        <v>-1.143908310661412</v>
       </c>
       <c r="J4">
-        <v>4.188218804692345</v>
+        <v>3.821414296213102</v>
       </c>
       <c r="K4">
-        <v>34.64966367515446</v>
+        <v>38.16961098865586</v>
       </c>
       <c r="L4">
         <v>-1.838999630883173</v>
       </c>
       <c r="M4">
-        <v>0.5030338931355397</v>
+        <v>0.5145224322936108</v>
       </c>
       <c r="N4">
-        <v>2.684002035969393E-13</v>
+        <v>7.644212961094954E-14</v>
       </c>
       <c r="O4">
-        <v>4.026003053954089E-13</v>
+        <v>1.146631944164243E-13</v>
       </c>
       <c r="P4">
-        <v>7.38100559891583E-13</v>
+        <v>2.102158564301112E-13</v>
       </c>
       <c r="Q4">
-        <v>171.259527360606</v>
+        <v>182.313992429254</v>
       </c>
       <c r="R4">
-        <v>66.7923224412523</v>
+        <v>81.80438360225391</v>
       </c>
       <c r="S4">
-        <v>59.90014389268</v>
+        <v>46.688636440254</v>
       </c>
       <c r="T4">
-        <v>200.872280227477</v>
+        <v>188.017261450254</v>
       </c>
       <c r="U4">
-        <v>153.319906098822</v>
+        <v>163.39630215502</v>
       </c>
       <c r="V4">
-        <v>149.886477756344</v>
+        <v>163.64887717302</v>
       </c>
       <c r="W4">
-        <v>155.69353201167</v>
+        <v>143.32714476502</v>
       </c>
       <c r="X4">
-        <v>180.263493815244</v>
+        <v>168.79108558902</v>
       </c>
       <c r="Y4">
-        <v>-160.095342837962</v>
+        <v>-150.997015794213</v>
       </c>
       <c r="Z4">
-        <v>-66.25742401256311</v>
+        <v>-53.7446863402134</v>
       </c>
       <c r="AA4">
-        <v>-210.14436207134</v>
+        <v>-221.665629112213</v>
       </c>
       <c r="AB4">
-        <v>-265.307061194989</v>
+        <v>-275.396858870213</v>
       </c>
       <c r="AC4">
-        <v>-90.9634409827455</v>
+        <v>-82.84318295144701</v>
       </c>
       <c r="AD4">
-        <v>-72.9087245514709</v>
+        <v>-61.6456486234471</v>
       </c>
       <c r="AE4">
-        <v>2.51853654365004</v>
+        <v>-8.157610291447099</v>
       </c>
       <c r="AF4">
-        <v>-93.2871251332224</v>
+        <v>-101.994312257447</v>
       </c>
       <c r="AG4">
-        <v>-196.657632662529</v>
+        <v>-189.515443643681</v>
       </c>
       <c r="AH4">
-        <v>-129.510058255378</v>
+        <v>-119.496644071681</v>
       </c>
       <c r="AI4">
-        <v>-230.00197419936</v>
+        <v>-239.833000828681</v>
       </c>
       <c r="AJ4">
-        <v>-182.653008976455</v>
+        <v>-189.977585549681</v>
       </c>
       <c r="AK4">
-        <v>-157.167715969313</v>
+        <v>-151.003595962914</v>
       </c>
       <c r="AL4">
-        <v>-199.229653575286</v>
+        <v>-190.465901135914</v>
       </c>
       <c r="AM4">
-        <v>-112.53952625437</v>
+        <v>-121.525432677914</v>
       </c>
       <c r="AN4">
-        <v>-187.140784332689</v>
+        <v>-193.082750354914</v>
       </c>
       <c r="AO4">
-        <v>-206.662793195097</v>
+        <v>-201.476742201148</v>
       </c>
       <c r="AP4">
-        <v>-168.142102005194</v>
+        <v>-160.628011310148</v>
       </c>
       <c r="AQ4">
-        <v>-164.53653918638</v>
+        <v>-172.677325404148</v>
       </c>
       <c r="AR4">
-        <v>-107.295481503922</v>
+        <v>-111.854836975148</v>
       </c>
       <c r="AS4">
-        <v>113.095467388119</v>
+        <v>117.303449369618</v>
       </c>
       <c r="AT4">
-        <v>134.703266493898</v>
+        <v>140.967695444618</v>
       </c>
       <c r="AU4">
-        <v>143.86714860461</v>
+        <v>136.571482592618</v>
       </c>
       <c r="AV4">
-        <v>160.541094435845</v>
+        <v>157.364349515618</v>
       </c>
       <c r="AW4">
-        <v>179.438096521335</v>
+        <v>182.668009490385</v>
       </c>
       <c r="AX4">
-        <v>187.999434429991</v>
+        <v>193.014201636385</v>
       </c>
       <c r="AY4">
-        <v>242.2898973986</v>
+        <v>235.839351592385</v>
       </c>
       <c r="AZ4">
-        <v>170.859454306612</v>
+        <v>169.065319937385</v>
       </c>
       <c r="BA4">
-        <v>163.203552122552</v>
+        <v>165.455396079151</v>
       </c>
       <c r="BB4">
-        <v>161.787254401083</v>
+        <v>165.552359863151</v>
       </c>
       <c r="BC4">
-        <v>148.28058816759</v>
+        <v>142.675162567151</v>
       </c>
       <c r="BD4">
-        <v>171.150664159379</v>
+        <v>170.739140341151</v>
       </c>
       <c r="BE4">
-        <v>291.238606859768</v>
+        <v>292.512381803917</v>
       </c>
       <c r="BF4">
-        <v>266.902745225175</v>
+        <v>269.418188942917</v>
       </c>
       <c r="BG4">
-        <v>220.02695785458</v>
+        <v>215.266652459917</v>
       </c>
       <c r="BH4">
-        <v>209.949398699146</v>
+        <v>210.920485431917</v>
       </c>
       <c r="BI4">
-        <v>280.119684032984</v>
+        <v>280.415389964684</v>
       </c>
       <c r="BJ4">
-        <v>295.974779430268</v>
+        <v>297.240561403684</v>
       </c>
       <c r="BK4">
-        <v>296.07335857557</v>
+        <v>292.158173386684</v>
       </c>
       <c r="BL4">
-        <v>206.633790376913</v>
+        <v>208.987487660684</v>
       </c>
       <c r="BM4">
-        <v>9.321191113199919</v>
+        <v>8.638828032449959</v>
       </c>
       <c r="BN4">
-        <v>-9.14355971664008</v>
+        <v>-9.12743948754996</v>
       </c>
       <c r="BO4">
-        <v>-7.81836193643994</v>
+        <v>-10.8884269195499</v>
       </c>
       <c r="BP4">
-        <v>-13.0795699383202</v>
+        <v>-9.34326210355005</v>
       </c>
       <c r="BQ4">
-        <v>26.357345099416</v>
+        <v>24.6969130062163</v>
       </c>
       <c r="BR4">
-        <v>-62.3664093175478</v>
+        <v>-63.5999508327836</v>
       </c>
       <c r="BS4">
-        <v>28.84080234755</v>
+        <v>26.6158575702163</v>
       </c>
       <c r="BT4">
-        <v>-20.5661849045532</v>
+        <v>-15.4472665187836</v>
       </c>
       <c r="BU4">
-        <v>-195.608544069368</v>
+        <v>-198.247045175017</v>
       </c>
       <c r="BV4">
-        <v>-208.941532947455</v>
+        <v>-211.424736207017</v>
       </c>
       <c r="BW4">
-        <v>-7.11026826445993</v>
+        <v>-8.490092836017309</v>
       </c>
       <c r="BX4">
-        <v>-62.8530237517863</v>
+        <v>-56.3514948150173</v>
       </c>
       <c r="BY4">
-        <v>-101.934248321152</v>
+        <v>-105.550818439251</v>
       </c>
       <c r="BZ4">
-        <v>-181.835361266363</v>
+        <v>-185.568226270251</v>
       </c>
       <c r="CA4">
-        <v>-224.60452035147</v>
+        <v>-225.139224717251</v>
       </c>
       <c r="CB4">
-        <v>-217.666333931019</v>
+        <v>-209.782194443251</v>
       </c>
       <c r="CC4">
-        <v>-214.648930748936</v>
+        <v>-219.243569879485</v>
       </c>
       <c r="CD4">
-        <v>-238.060178341271</v>
+        <v>-243.042705089485</v>
       </c>
       <c r="CE4">
-        <v>-240.04657769848</v>
+        <v>-239.736161858485</v>
       </c>
       <c r="CF4">
-        <v>-98.6984901562524</v>
+        <v>-89.43174011748469</v>
       </c>
       <c r="CG4">
-        <v>-249.908707927719</v>
+        <v>-255.481416070718</v>
       </c>
       <c r="CH4">
-        <v>-124.463093298178</v>
+        <v>-130.695281790718</v>
       </c>
       <c r="CI4">
-        <v>-238.87303049449</v>
+        <v>-237.717494448718</v>
       </c>
       <c r="CJ4">
-        <v>-216.956844750486</v>
+        <v>-206.307484160718</v>
       </c>
       <c r="CK4">
-        <v>-158.227252530503</v>
+        <v>-164.778029685952</v>
       </c>
       <c r="CL4">
-        <v>-223.357840078086</v>
+        <v>-230.839690314952</v>
       </c>
       <c r="CM4">
-        <v>-186.5198085905</v>
+        <v>-184.519152338952</v>
       </c>
       <c r="CN4">
-        <v>-57.3467091087185</v>
+        <v>-45.3147379679518</v>
       </c>
       <c r="CO4">
-        <v>-15.084223690287</v>
+        <v>-22.6130698581856</v>
       </c>
       <c r="CP4">
-        <v>15.9430163460061</v>
+        <v>7.21150436481446</v>
       </c>
       <c r="CQ4">
-        <v>0.568501011489957</v>
+        <v>3.41427746881436</v>
       </c>
       <c r="CR4">
-        <v>-2.69908768095172</v>
+        <v>10.7154940108144</v>
       </c>
       <c r="CS4">
-        <v>-9.838553052070781</v>
+        <v>-18.3454682324192</v>
       </c>
       <c r="CT4">
-        <v>3.72450887009836</v>
+        <v>-6.25666485541922</v>
       </c>
       <c r="CU4">
-        <v>-13.7213294345199</v>
+        <v>-10.0304327714192</v>
       </c>
       <c r="CV4">
-        <v>-97.1817660451848</v>
+        <v>-82.3845738024193</v>
       </c>
       <c r="CW4">
-        <v>106.153443319145</v>
+        <v>96.6684591263471</v>
       </c>
       <c r="CX4">
-        <v>117.199216234191</v>
+        <v>105.968380764347</v>
       </c>
       <c r="CY4">
-        <v>83.61996038146999</v>
+        <v>88.15597725034711</v>
       </c>
       <c r="CZ4">
-        <v>82.38179601858219</v>
+        <v>98.5615988123471</v>
       </c>
       <c r="DA4">
-        <v>89.7664155503613</v>
+        <v>79.3033623451133</v>
       </c>
       <c r="DB4">
-        <v>129.702172865283</v>
+        <v>117.221675651113</v>
       </c>
       <c r="DC4">
-        <v>63.7515844914601</v>
+        <v>69.1327215661134</v>
       </c>
       <c r="DD4">
-        <v>60.6469785663492</v>
+        <v>78.2093919111135</v>
       </c>
       <c r="DE4">
-        <v>-21.1626475164225</v>
+        <v>-32.6037697341203</v>
       </c>
       <c r="DF4">
-        <v>-36.6598184286247</v>
+        <v>-50.3899773871202</v>
       </c>
       <c r="DG4">
-        <v>30.1577503864502</v>
+        <v>36.3840076668798</v>
       </c>
       <c r="DH4">
-        <v>-30.0376909358839</v>
+        <v>-11.0926670401202</v>
       </c>
       <c r="DI4">
-        <v>194.686798037794</v>
+        <v>182.267606807646</v>
       </c>
       <c r="DJ4">
-        <v>190.260561300468</v>
+        <v>175.280740597646</v>
       </c>
       <c r="DK4">
-        <v>160.32753681444</v>
+        <v>167.398914300646</v>
       </c>
       <c r="DL4">
-        <v>209.470211738883</v>
+        <v>229.797846185646</v>
       </c>
       <c r="DM4">
-        <v>371.5707420886988</v>
+        <v>332.2853091897304</v>
       </c>
       <c r="DN4">
-        <v>144.5206153564815</v>
+        <v>141.767039711691</v>
       </c>
       <c r="DO4">
-        <v>-64.24179900194748</v>
+        <v>-46.82637389212259</v>
       </c>
       <c r="DP4">
-        <v>-191.1684863114423</v>
+        <v>-172.8625641207078</v>
       </c>
       <c r="DQ4">
-        <v>-214.4484415032709</v>
+        <v>-207.2147930731664</v>
       </c>
       <c r="DR4">
-        <v>-151.1709853278683</v>
+        <v>-155.8227861922032</v>
       </c>
       <c r="DS4">
-        <v>-42.51182225110855</v>
+        <v>-51.25106683254111</v>
       </c>
       <c r="DT4">
-        <v>65.39018167734488</v>
+        <v>62.79328528521164</v>
       </c>
       <c r="DU4">
-        <v>137.6204140612847</v>
+        <v>147.6673307656817</v>
       </c>
       <c r="DV4">
-        <v>159.173749146822</v>
+        <v>181.347529876626</v>
       </c>
       <c r="DW4">
-        <v>135.0977773955838</v>
+        <v>162.461600998207</v>
       </c>
       <c r="DX4">
-        <v>84.07987700621062</v>
+        <v>106.892106277142</v>
       </c>
       <c r="DY4">
-        <v>29.12384174245835</v>
+        <v>39.43147471488066</v>
       </c>
       <c r="DZ4">
-        <v>-10.95904672423938</v>
+        <v>-15.89259756816869</v>
       </c>
       <c r="EA4">
-        <v>-26.6707854628951</v>
+        <v>-43.44539569026199</v>
       </c>
       <c r="EB4">
-        <v>-18.69990130435443</v>
+        <v>-39.48066930310418</v>
       </c>
       <c r="EC4">
-        <v>4.726208717239373</v>
+        <v>-11.14143472178436</v>
       </c>
       <c r="ED4">
-        <v>32.31096187287037</v>
+        <v>27.87495942786288</v>
       </c>
       <c r="EE4">
-        <v>54.09302815223113</v>
+        <v>62.9653069773765</v>
       </c>
       <c r="EF4">
-        <v>64.36851795602313</v>
+        <v>83.51160741086309</v>
       </c>
       <c r="EG4">
-        <v>62.53316465721096</v>
+        <v>85.57381300732632</v>
       </c>
       <c r="EH4">
-        <v>52.06548824303313</v>
+        <v>71.92222483613511</v>
       </c>
       <c r="EI4">
-        <v>38.42398587579201</v>
+        <v>49.89376643223321</v>
       </c>
       <c r="EJ4">
-        <v>26.80067068393643</v>
+        <v>28.17006787347608</v>
       </c>
       <c r="EK4">
-        <v>20.49579237580277</v>
+        <v>13.71980882993632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds ion trace toggle to tab 3
</commit_message>
<xml_diff>
--- a/ion_rhythmicity.xlsx
+++ b/ion_rhythmicity.xlsx
@@ -354,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -363,30 +363,25 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>rowname</t>
+          <t>Ion</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Ion</t>
+          <t>pVal</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>pVal</t>
+          <t>phase</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>phase</t>
+          <t>peak.shape</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>peak.shape</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>period</t>
         </is>
@@ -395,96 +390,57 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
+          <t>Mg</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>0.004613852787293322</v>
       </c>
       <c r="C2">
-        <v>4.189047761245855E-21</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
         <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Mg</t>
-        </is>
+          <t>Ca</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.004263315365191727</v>
       </c>
       <c r="C3">
-        <v>0.004613852787293322</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>18</v>
-      </c>
-      <c r="F3">
         <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Ca</t>
-        </is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>1.345439998676246E-11</v>
       </c>
       <c r="C4">
-        <v>0.004263315365191727</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E4">
-        <v>18</v>
-      </c>
-      <c r="F4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>1.345439998676246E-11</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>16</v>
-      </c>
-      <c r="F5">
         <v>24</v>
       </c>
     </row>
@@ -495,7 +451,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -504,30 +460,25 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>rowname</t>
+          <t>Ion</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Ion</t>
+          <t>pVal</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>pVal</t>
+          <t>phase</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>phase</t>
+          <t>peak.shape</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>peak.shape</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>period</t>
         </is>
@@ -536,96 +487,57 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Time</t>
-        </is>
+          <t>Mg</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>2.917243396018233E-31</v>
       </c>
       <c r="C2">
-        <v>2.894257498096193E-45</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Mg</t>
-        </is>
+          <t>Ca</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>0.0001298639475702177</v>
       </c>
       <c r="C3">
-        <v>2.917243396018233E-31</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Ca</t>
-        </is>
+          <t>K</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>2.760357753881839E-24</v>
       </c>
       <c r="C4">
-        <v>0.0001298639475702177</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>2.760357753881839E-24</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
-      </c>
-      <c r="F5">
         <v>26</v>
       </c>
     </row>

</xml_diff>